<commit_message>
Added login, menu and products Test
</commit_message>
<xml_diff>
--- a/softinnovas/Data_Test_Swag_Web_Site.xlsx
+++ b/softinnovas/Data_Test_Swag_Web_Site.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kayru\eclipse-workspace\selenium\java-selenium-learning\softinnovas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777A6686-7390-43C1-AB84-096ECF31B756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6917D8DE-67E3-49F4-90B4-26F147139DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{296ADB0E-561D-4BE5-9EA7-FB128B7DC767}"/>
+    <workbookView xWindow="4812" yWindow="4812" windowWidth="23040" windowHeight="13560" activeTab="1" xr2:uid="{296ADB0E-561D-4BE5-9EA7-FB128B7DC767}"/>
   </bookViews>
   <sheets>
     <sheet name="login_cases" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
     <t>test_type</t>
   </si>
   <si>
-    <t>Amount_Item</t>
+    <t>Amount_Items</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F83794-539E-4608-ACF0-8543E07456CD}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -671,9 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4227A099-50C6-4682-A810-BD117352A2BE}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Added save printscreen in reporter
added printscreen to reporter
change some xpath
remove severall Assert
Separate data test in diferents files
</commit_message>
<xml_diff>
--- a/softinnovas/Data_Test_Swag_Web_Site.xlsx
+++ b/softinnovas/Data_Test_Swag_Web_Site.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kayru\eclipse-workspace\selenium\java-selenium-learning\softinnovas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142839E6-07F8-4402-9E9F-D64E2AE9A189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BCA296-2CBB-4F3C-BCEC-2679EF016EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{296ADB0E-561D-4BE5-9EA7-FB128B7DC767}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{296ADB0E-561D-4BE5-9EA7-FB128B7DC767}"/>
   </bookViews>
   <sheets>
     <sheet name="login_cases" sheetId="1" r:id="rId1"/>
-    <sheet name="Shopping_items" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>user</t>
   </si>
@@ -91,18 +90,6 @@
   </si>
   <si>
     <t>test_type</t>
-  </si>
-  <si>
-    <t>Item_Names</t>
-  </si>
-  <si>
-    <t>Sauce Labs Bolt T-Shirt</t>
-  </si>
-  <si>
-    <t>Sauce Labs Bike Light</t>
-  </si>
-  <si>
-    <t>Remove</t>
   </si>
 </sst>
 </file>
@@ -487,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F83794-539E-4608-ACF0-8543E07456CD}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -674,45 +661,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4227A099-50C6-4682-A810-BD117352A2BE}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>